<commit_message>
add abas de notas e bens
</commit_message>
<xml_diff>
--- a/ORGANIZADOR DECLARAÇÃO IR.xlsx
+++ b/ORGANIZADOR DECLARAÇÃO IR.xlsx
@@ -5,25 +5,26 @@
   <workbookPr codeName="EstaPastaDeTrabalho"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arquivos_Sistema\Downloads\ORGANIZADOR IR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arquivos_Sistema\Downloads\ORGANIZADOR IR\Organizador-IR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4E5720-24F3-4AD6-ACE6-7172D846C940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCC3980-89FA-4D57-BB7B-935466212796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TITULAR" sheetId="1" r:id="rId1"/>
     <sheet name="INFORMES" sheetId="7" r:id="rId2"/>
     <sheet name="NOTAS" sheetId="8" r:id="rId3"/>
-    <sheet name="TABELAS" sheetId="9" r:id="rId4"/>
+    <sheet name="BENS E DIREITOS" sheetId="11" r:id="rId4"/>
+    <sheet name="TABELAS" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="185">
   <si>
     <t>1. DADOS DO TÍTULAR</t>
   </si>
@@ -265,9 +266,6 @@
     <t>PRÓXIMO ➡️</t>
   </si>
   <si>
-    <t>3. NOTAS BANCÁRIAS OU EXTRATO DE OLHERITES</t>
-  </si>
-  <si>
     <t>2. INFORMES DE RENDIMENTOS BANCÁRIOS</t>
   </si>
   <si>
@@ -281,19 +279,322 @@
   </si>
   <si>
     <t>ENTRADAS</t>
+  </si>
+  <si>
+    <t>São todos os valores de entrada de receita mês a mês</t>
+  </si>
+  <si>
+    <t>3. NOTAS BANCÁRIAS OU EXTRATO DE HOLHERITES</t>
+  </si>
+  <si>
+    <t>HOLHERITE</t>
+  </si>
+  <si>
+    <t>SAÍDAS</t>
+  </si>
+  <si>
+    <t>4. NOTAS E DESPESAS DEDUTÍVEIS</t>
+  </si>
+  <si>
+    <t>DESPESAS DEDUTÍVEIS</t>
+  </si>
+  <si>
+    <t>Exames laboratoriais e de imagem</t>
+  </si>
+  <si>
+    <t>Cirurgias</t>
+  </si>
+  <si>
+    <t>Internações hospitalares</t>
+  </si>
+  <si>
+    <t>Consultas médicas</t>
+  </si>
+  <si>
+    <t>Consultas odontológicas</t>
+  </si>
+  <si>
+    <t>Consultas psicológicas, psiquiátricas e terapêuticas</t>
+  </si>
+  <si>
+    <t>Mensalidades de plano de saúde</t>
+  </si>
+  <si>
+    <t>Coparticipações de plano de saúde</t>
+  </si>
+  <si>
+    <t>Próteses e aparelhos ortopédicos ou dentários vinculados a procedimentos médicos</t>
+  </si>
+  <si>
+    <t>Educação infantil (creche e pré-escola)</t>
+  </si>
+  <si>
+    <t>Ensino fundamental</t>
+  </si>
+  <si>
+    <t>Ensino médio</t>
+  </si>
+  <si>
+    <t>Ensino técnico</t>
+  </si>
+  <si>
+    <t>Ensino superior (graduação)</t>
+  </si>
+  <si>
+    <t>Pós-graduação (especialização, mestrado e doutorado)</t>
+  </si>
+  <si>
+    <t>Dedução anual por dependente</t>
+  </si>
+  <si>
+    <t>Despesas médicas de dependentes</t>
+  </si>
+  <si>
+    <t>Despesas educacionais de dependentes</t>
+  </si>
+  <si>
+    <t>Pensão alimentícia determinada por decisão judicial ou escritura pública</t>
+  </si>
+  <si>
+    <t>Despesas obrigatórias previstas na pensão alimentícia (escola e plano de saúde)</t>
+  </si>
+  <si>
+    <t>Contribuições à Previdência Social – INSS</t>
+  </si>
+  <si>
+    <t>Contribuições à previdência privada do tipo PGBL (limitadas a 12% da renda tributável anual)</t>
+  </si>
+  <si>
+    <t>Doações aos Fundos dos Direitos da Criança e do Adolescente</t>
+  </si>
+  <si>
+    <t>Doações aos Fundos dos Direitos do Idoso</t>
+  </si>
+  <si>
+    <t>Doações a projetos culturais (Lei Rouanet)</t>
+  </si>
+  <si>
+    <t>Doações a projetos audiovisuais</t>
+  </si>
+  <si>
+    <t>Doações a projetos esportivos</t>
+  </si>
+  <si>
+    <t>Doações aos programas PRONON</t>
+  </si>
+  <si>
+    <t>Doações aos programas PRONAS/PCD</t>
+  </si>
+  <si>
+    <t>Contribuição patronal ao INSS de empregado doméstico</t>
+  </si>
+  <si>
+    <t>Honorários advocatícios relacionados a ações trabalhistas</t>
+  </si>
+  <si>
+    <t>Honorários advocatícios relacionados a ações previdenciárias</t>
+  </si>
+  <si>
+    <t>Honorários advocatícios vinculados ao recebimento de rendimentos tributáveis</t>
+  </si>
+  <si>
+    <t>São todos os valores de despesas dedutíveis</t>
+  </si>
+  <si>
+    <t>5. BENS E DIREITOS</t>
+  </si>
+  <si>
+    <t>CÓDIGO</t>
+  </si>
+  <si>
+    <t>VALOR DATA INICIAL</t>
+  </si>
+  <si>
+    <t>VALOR DATA FINAL</t>
+  </si>
+  <si>
+    <t>BENS E DIREITOS</t>
+  </si>
+  <si>
+    <t>Código 11 – Apartamento</t>
+  </si>
+  <si>
+    <t>Código 12 – Casa</t>
+  </si>
+  <si>
+    <t>Código 13 – Terreno</t>
+  </si>
+  <si>
+    <t>Código 15 – Sala ou conjunto comercial</t>
+  </si>
+  <si>
+    <t>Código 16 – Construção</t>
+  </si>
+  <si>
+    <t>Código 17 – Benfeitorias</t>
+  </si>
+  <si>
+    <t>Código 18 – Outros bens imóveis</t>
+  </si>
+  <si>
+    <t>GRUPO 01 - Bens Imóveis</t>
+  </si>
+  <si>
+    <t>GRUPO 02 – Bens Móveis</t>
+  </si>
+  <si>
+    <t>Código 01 – Veículo automotor terrestre</t>
+  </si>
+  <si>
+    <t>Código 02 – Aeronave</t>
+  </si>
+  <si>
+    <t>Código 03 – Embarcação</t>
+  </si>
+  <si>
+    <t>Código 99 – Outros bens móveis</t>
+  </si>
+  <si>
+    <t>GRUPO 01 – Bens Imóveis</t>
+  </si>
+  <si>
+    <t>GRUPO 03 – Participações Societárias</t>
+  </si>
+  <si>
+    <t>Código 01 – Ações (inclusive as negociadas em bolsa)</t>
+  </si>
+  <si>
+    <t>Código 02 – Quotas ou quinhões de capital</t>
+  </si>
+  <si>
+    <t>Código 03 – Outros investimentos societários</t>
+  </si>
+  <si>
+    <t>GRUPO 04 – Aplicações e Investimentos</t>
+  </si>
+  <si>
+    <t>Código 01 – Caderneta de poupança</t>
+  </si>
+  <si>
+    <t>Código 02 – CDB, RDB e outros títulos bancários</t>
+  </si>
+  <si>
+    <t>Código 03 – Tesouro Direto</t>
+  </si>
+  <si>
+    <t>Código 04 – Fundos de investimento</t>
+  </si>
+  <si>
+    <t>Código 05 – Letras de crédito (LCI e LCA)</t>
+  </si>
+  <si>
+    <t>Código 06 – Certificados de recebíveis (CRI e CRA)</t>
+  </si>
+  <si>
+    <t>Código 99 – Outros investimentos</t>
+  </si>
+  <si>
+    <t>GRUPO 05 – Créditos</t>
+  </si>
+  <si>
+    <t>Código 01 – Crédito decorrente de empréstimo</t>
+  </si>
+  <si>
+    <t>Código 02 – Crédito decorrente de venda a prazo</t>
+  </si>
+  <si>
+    <t>Código 99 – Outros créditos</t>
+  </si>
+  <si>
+    <t>GRUPO 06 – Depósitos à Vista e Numerário</t>
+  </si>
+  <si>
+    <t>Código 01 – Dinheiro em espécie</t>
+  </si>
+  <si>
+    <t>Código 02 – Conta corrente</t>
+  </si>
+  <si>
+    <t>Código 03 – Conta pagamento (fintechs e bancos digitais)</t>
+  </si>
+  <si>
+    <t>GRUPO 07 – Fundos</t>
+  </si>
+  <si>
+    <t>Código 01 – Fundos de investimento imobiliário (FII)</t>
+  </si>
+  <si>
+    <t>Código 02 – Fundos de ações</t>
+  </si>
+  <si>
+    <t>Código 03 – Fundos multimercado</t>
+  </si>
+  <si>
+    <t>Código 99 – Outros fundos</t>
+  </si>
+  <si>
+    <t>GRUPO 08 – Criptoativos</t>
+  </si>
+  <si>
+    <t>Código 01 – Bitcoin (BTC)</t>
+  </si>
+  <si>
+    <t>Código 02 – Outras criptomoedas</t>
+  </si>
+  <si>
+    <t>Código 03 – Tokens</t>
+  </si>
+  <si>
+    <t>Código 10 – NFTs</t>
+  </si>
+  <si>
+    <t>GRUPO 09 – Outros Bens e Direitos</t>
+  </si>
+  <si>
+    <t>Código 01 – Consórcio não contemplado</t>
+  </si>
+  <si>
+    <t>Código 02 – Consórcio contemplado</t>
+  </si>
+  <si>
+    <t>Código 03 – Direitos autorais</t>
+  </si>
+  <si>
+    <t>Código 04 – Patentes e marcas</t>
+  </si>
+  <si>
+    <t>Código 99 – Outros bens e direitos</t>
+  </si>
+  <si>
+    <t>DESCRIÇÃO</t>
+  </si>
+  <si>
+    <t>GRUPO 02 - Bens Móveis</t>
+  </si>
+  <si>
+    <t>TOTAL DATA INICIAL</t>
+  </si>
+  <si>
+    <t>TOTAL DATA FINAL</t>
+  </si>
+  <si>
+    <t>São todos os valores referentes a bens e direitos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="9">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="000&quot;.&quot;000&quot;.&quot;000&quot;-&quot;00"/>
     <numFmt numFmtId="165" formatCode="&quot;(&quot;00&quot;)&quot;00000&quot;-&quot;0000"/>
     <numFmt numFmtId="166" formatCode="&quot;(&quot;00&quot;)&quot;0000&quot;-&quot;0000"/>
     <numFmt numFmtId="167" formatCode="00&quot;/&quot;00&quot;/&quot;0000"/>
     <numFmt numFmtId="168" formatCode="00000\-000"/>
     <numFmt numFmtId="169" formatCode="[$R$-416]\ #,##0.00;\-[$R$-416]\ #,##0.00"/>
+    <numFmt numFmtId="171" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="172" formatCode="mmmm\-yyyy"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -318,12 +619,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -401,8 +696,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -457,8 +758,20 @@
         <bgColor rgb="FFFFE599"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -616,36 +929,31 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color theme="1"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -656,50 +964,50 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="169" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -708,53 +1016,200 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Moeda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="13">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="171" formatCode="&quot;R$&quot;\ #,##0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="171" formatCode="&quot;R$&quot;\ #,##0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1292,6 +1747,108 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>866775</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2876550</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="CaixaDeTexto 2">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB792B3B-FDD3-47D3-A97A-6D4418A74F53}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="866775" y="7400925"/>
+          <a:ext cx="2009775" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="5000"/>
+                <a:lumOff val="95000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="74000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="45000"/>
+                <a:lumOff val="55000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="83000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="45000"/>
+                <a:lumOff val="55000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="30000"/>
+                <a:lumOff val="70000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="1" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>BENS E DIREITOS</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1366,15 +1923,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>857250</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2886075</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>2867025</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1390,7 +1947,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="876300" y="5619750"/>
+          <a:off x="857250" y="5800725"/>
           <a:ext cx="2009775" cy="352425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1468,15 +2025,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>866775</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>857250</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2876550</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:colOff>2867025</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1492,7 +2049,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="866775" y="6238875"/>
+          <a:off x="857250" y="6305550"/>
           <a:ext cx="2009775" cy="352425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1544,15 +2101,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>847725</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>857250</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2857500</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>2867025</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1568,7 +2125,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="847725" y="6848475"/>
+          <a:off x="857250" y="6819900"/>
           <a:ext cx="2009775" cy="352425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1816,6 +2373,108 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>847725</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="CaixaDeTexto 7">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08A54B10-67DC-4C0D-98EB-26FB7F462634}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="847725" y="7353300"/>
+          <a:ext cx="2009775" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="5000"/>
+                <a:lumOff val="95000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="74000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="45000"/>
+                <a:lumOff val="55000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="83000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="45000"/>
+                <a:lumOff val="55000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="30000"/>
+                <a:lumOff val="70000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="1" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>BENS E DIREITOS</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2182,7 +2841,7 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2781300</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2347,11 +3006,781 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>857250</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2867025</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="CaixaDeTexto 7">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FDB66B2-EF24-480D-9686-EA20451B9A81}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="857250" y="7439025"/>
+          <a:ext cx="2009775" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="5000"/>
+                <a:lumOff val="95000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="74000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="45000"/>
+                <a:lumOff val="55000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="83000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="45000"/>
+                <a:lumOff val="55000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="30000"/>
+                <a:lumOff val="70000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="1" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>BENS E DIREITOS</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3724275" cy="8296275"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="image1.png" title="Imagem">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{803CD806-55F8-4E74-A25B-D233DE4CD535}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="3724275" cy="8296275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="5000"/>
+                <a:lumOff val="95000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="74000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="45000"/>
+                <a:lumOff val="55000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="83000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="45000"/>
+                <a:lumOff val="55000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="30000"/>
+                <a:lumOff val="70000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>876300</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2886075</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="CaixaDeTexto 2">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA9427B6-5CF9-4C85-8FE1-471F56E421EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="876300" y="5619750"/>
+          <a:ext cx="2009775" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="5000"/>
+                <a:lumOff val="95000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="74000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="45000"/>
+                <a:lumOff val="55000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="83000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="45000"/>
+                <a:lumOff val="55000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="30000"/>
+                <a:lumOff val="70000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="1" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>TITULAR</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>866775</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2876550</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="CaixaDeTexto 3">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A9C1BDA-01FD-4517-9D77-405646D891D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="866775" y="6238875"/>
+          <a:ext cx="2009775" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="5000"/>
+                <a:lumOff val="95000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="74000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="45000"/>
+                <a:lumOff val="55000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="83000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="45000"/>
+                <a:lumOff val="55000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="30000"/>
+                <a:lumOff val="70000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="1" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>INFORMES</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>847725</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="CaixaDeTexto 4">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C998E3D-D11F-474D-BA28-44FB9A7F552D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="847725" y="6848475"/>
+          <a:ext cx="2009775" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="5000"/>
+                <a:lumOff val="95000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="74000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="45000"/>
+                <a:lumOff val="55000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="83000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="45000"/>
+                <a:lumOff val="55000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent1">
+                <a:lumMod val="30000"/>
+                <a:lumOff val="70000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="1"/>
+        </a:gradFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="1" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>NOTAS</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>942975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2781300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="CaixaDeTexto 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B580D9FF-DCCA-4E2A-9836-ED2E48CC9189}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="942975" y="0"/>
+          <a:ext cx="1838325" cy="523875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill flip="none" rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="35455">
+              <a:srgbClr val="FFFFFD"/>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="accent3">
+                <a:lumMod val="0"/>
+                <a:lumOff val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="89000">
+              <a:schemeClr val="accent3">
+                <a:lumMod val="0"/>
+                <a:lumOff val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent3">
+                <a:lumMod val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+          <a:tileRect/>
+        </a:gradFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1000" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>SYSTEM</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1000" b="1" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> BY SAMARA </a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1000" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2524126</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2733676</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>51435</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagem 6" descr="LinkedIn">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9CBA33B-2606-42E1-97F0-AFFBBE4639FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="59542" t="-2085" r="13741" b="14565"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2524126" y="0"/>
+          <a:ext cx="209550" cy="251460"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2847975</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="CaixaDeTexto 7">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF04B6CF-7613-4452-AC03-F793EBF3EA2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="838200" y="7439025"/>
+          <a:ext cx="2009775" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="1" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx2"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>BENS E DIREITOS</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <x18tc:personList xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments"/>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{484F905B-6042-4191-8C58-8AB7B828F4C3}" name="Tabela1" displayName="Tabela1" ref="C7:E48" totalsRowShown="0" dataDxfId="9">
+  <autoFilter ref="C7:E48" xr:uid="{484F905B-6042-4191-8C58-8AB7B828F4C3}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{8F7E4433-525E-40F6-9638-B77AA15FAE3D}" name="DATA" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{B11AC525-796F-4F62-BA1E-D9B4960DD205}" name="CATEGORIA" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{FA0C0CDB-D9D2-4E3D-829A-855A1FEEA23E}" name="VALOR" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{131852E7-40F2-482A-8B7F-F99139B8F1A0}" name="Tabela13" displayName="Tabela13" ref="G7:I48" totalsRowShown="0" dataDxfId="8">
+  <autoFilter ref="G7:I48" xr:uid="{131852E7-40F2-482A-8B7F-F99139B8F1A0}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{560CE083-D6F2-4502-A268-B7809B624E6B}" name="DATA" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{1B3AE8EC-0B18-4A0A-81B3-3ACC655D3395}" name="CATEGORIA" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{6845F245-FBFD-4F2F-9DB9-07AA42FBD895}" name="VALOR" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F73AAB36-4E48-4471-A257-9B5DE2776EAC}" name="Tabela14" displayName="Tabela14" ref="C7:F75" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="C7:F75" xr:uid="{484F905B-6042-4191-8C58-8AB7B828F4C3}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{AF424B4B-B374-4EF5-92E3-62EF0305F9D4}" name="GRUPO 01 - Bens Imóveis" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{BE076784-716F-4346-A89D-4DF666113EFB}" name="DESCRIÇÃO" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{0FE057A0-F2EE-4519-B2E5-FDE90B76F343}" name="VALOR DATA INICIAL" dataDxfId="0" dataCellStyle="Moeda"/>
+    <tableColumn id="3" xr3:uid="{A0812ADF-AD83-4700-A19D-75CF2121FC46}" name="VALOR DATA FINAL" dataDxfId="1" dataCellStyle="Moeda"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2557,9 +3986,7 @@
   </sheetPr>
   <dimension ref="C2:D20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2574,117 +4001,117 @@
       </c>
     </row>
     <row r="3" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="26"/>
+      <c r="D3" s="31"/>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>12345647889</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="12">
         <v>25021999</v>
       </c>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="7">
         <v>789456142</v>
       </c>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="7"/>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="8"/>
+      <c r="D11" s="7"/>
     </row>
     <row r="12" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="13">
         <v>63132085</v>
       </c>
     </row>
     <row r="13" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="11">
         <v>8899999999</v>
       </c>
     </row>
     <row r="14" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="10">
         <v>88995555555</v>
       </c>
     </row>
     <row r="15" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="26" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2713,9 +4140,7 @@
   </sheetPr>
   <dimension ref="C2:D33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
-    </sheetView>
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2724,122 +4149,122 @@
     <col min="3" max="4" width="43.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C2" s="32" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C3" s="27" t="s">
+    <row r="2" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C2" s="27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C3" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="28"/>
-    </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.2"/>
+      <c r="D3" s="33"/>
+    </row>
+    <row r="4" spans="3:4" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="5" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="24">
         <f>SUM(D10,D16,D22,D29)</f>
         <v>23570084</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:4" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="3:4" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C9" s="16" t="s">
+    <row r="9" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C9" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="20" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C10" s="17" t="s">
+    <row r="10" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C10" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="17">
         <v>5892521</v>
       </c>
     </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C11" s="22" t="s">
+    <row r="11" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C11" s="21" t="s">
         <v>23</v>
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C12" s="23"/>
-      <c r="D12" s="24"/>
-    </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C13" s="23"/>
-      <c r="D13" s="24"/>
-    </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C12" s="22"/>
+      <c r="D12" s="23"/>
+    </row>
+    <row r="13" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C13" s="22"/>
+      <c r="D13" s="23"/>
+    </row>
+    <row r="14" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C15" s="16" t="s">
+    <row r="15" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C15" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="20" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C16" s="17" t="s">
+    <row r="16" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C16" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="17">
         <v>5892521</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C17" s="22" t="s">
+    <row r="17" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C17" s="21" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C18" s="23"/>
-      <c r="D18" s="24"/>
-    </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C19" s="23"/>
-      <c r="D19" s="24"/>
+    <row r="18" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C18" s="22"/>
+      <c r="D18" s="23"/>
+    </row>
+    <row r="19" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C19" s="22"/>
+      <c r="D19" s="23"/>
     </row>
     <row r="20" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C21" s="16" t="s">
+    <row r="21" spans="3:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C21" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="D21" s="20" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="22" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="17">
         <v>5892521</v>
       </c>
     </row>
     <row r="23" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="21" t="s">
         <v>23</v>
       </c>
       <c r="D23" s="2"/>
@@ -2850,32 +4275,32 @@
       </c>
     </row>
     <row r="28" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D28" s="20" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="29" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="18">
+      <c r="D29" s="17">
         <v>5892521</v>
       </c>
     </row>
     <row r="30" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="21" t="s">
         <v>23</v>
       </c>
       <c r="D30" s="2"/>
     </row>
     <row r="33" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C33" s="31" t="s">
+      <c r="C33" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="D33" s="31" t="s">
+      <c r="D33" s="26" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2909,384 +4334,1617 @@
   <sheetPr codeName="Planilha4">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="C2:E20"/>
+  <dimension ref="C1:I48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="59.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="56" customWidth="1"/>
+    <col min="2" max="2" width="3.140625" customWidth="1"/>
     <col min="3" max="4" width="43.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="8" width="43.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C2" s="32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C5" s="34" t="s">
+    <row r="1" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C3" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C4" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C6" s="38" t="s">
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="G4" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C6" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="G6" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C7" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="E7" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="38" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C8" s="41"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="43"/>
-    </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C9" s="41"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="43"/>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C10" s="41"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="43"/>
-    </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C11" s="41"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="43"/>
-    </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C12" s="41"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="43"/>
-    </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C13" s="41"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="43"/>
-    </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C14" s="41"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="43"/>
-    </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C15" s="41"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="43"/>
-    </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C16" s="41"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="43"/>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C17" s="41"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="43"/>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C18" s="36"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="35"/>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C20" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="G7" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>82</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C8" s="38">
+        <v>45323</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="37">
+        <v>2500</v>
+      </c>
+      <c r="G8" s="38">
+        <v>45802</v>
+      </c>
+      <c r="H8" s="36"/>
+      <c r="I8" s="37">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C9" s="38"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="37"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="37"/>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C10" s="38"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="37"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="37"/>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C11" s="38"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="37"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="37"/>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C12" s="38"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="37"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="37"/>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C13" s="38"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="37"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="37"/>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C14" s="38"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="37"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="37"/>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C15" s="38"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="37"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="37"/>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C16" s="38"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="37"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="37"/>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C17" s="38"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="37"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="37"/>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C18" s="38"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="37"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="37"/>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C19" s="38"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="37"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="37"/>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C20" s="38"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="37"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="37"/>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C21" s="38"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="37"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="37"/>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C22" s="38"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="37"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="37"/>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C23" s="38"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="37"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="37"/>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C24" s="38"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="37"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="37"/>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C25" s="38"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="37"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="37"/>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C26" s="38"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="37"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="37"/>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C27" s="38"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="37"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="37"/>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C28" s="38"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="37"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="37"/>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C29" s="38"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="37"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="37"/>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C30" s="38"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="37"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="37"/>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C31" s="38"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="37"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="37"/>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C32" s="38"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="37"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="37"/>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C33" s="38"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="37"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="37"/>
+    </row>
+    <row r="34" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C34" s="38"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="37"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="36"/>
+      <c r="I34" s="37"/>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C35" s="38"/>
+      <c r="D35" s="36"/>
+      <c r="E35" s="37"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="36"/>
+      <c r="I35" s="37"/>
+    </row>
+    <row r="36" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C36" s="38"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="37"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="37"/>
+    </row>
+    <row r="37" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C37" s="38"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="37"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="37"/>
+    </row>
+    <row r="38" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C38" s="38"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="37"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="37"/>
+    </row>
+    <row r="39" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C39" s="38"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="37"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="37"/>
+    </row>
+    <row r="40" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C40" s="38"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="37"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="37"/>
+    </row>
+    <row r="41" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C41" s="38"/>
+      <c r="D41" s="36"/>
+      <c r="E41" s="37"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="36"/>
+      <c r="I41" s="37"/>
+    </row>
+    <row r="42" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C42" s="38"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="37"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="37"/>
+    </row>
+    <row r="43" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C43" s="38"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="37"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="37"/>
+    </row>
+    <row r="44" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C44" s="38"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="37"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="37"/>
+    </row>
+    <row r="45" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C45" s="38"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="37"/>
+      <c r="G45" s="38"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="37"/>
+    </row>
+    <row r="46" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C46" s="38"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="37"/>
+      <c r="G46" s="38"/>
+      <c r="H46" s="36"/>
+      <c r="I46" s="37"/>
+    </row>
+    <row r="47" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C47" s="38"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="37"/>
+      <c r="G47" s="38"/>
+      <c r="H47" s="36"/>
+      <c r="I47" s="37"/>
+    </row>
+    <row r="48" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C48" s="38"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="37"/>
+      <c r="G48" s="38"/>
+      <c r="H48" s="36"/>
+      <c r="I48" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C5:E5"/>
+  <mergeCells count="4">
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G4:I4"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D48" xr:uid="{2DA134E1-6EB5-43A8-9FE4-25F8FBF045F4}">
+      <formula1>"HOLHERITE,CNPJ,FREELANCE"</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C20" location="INFORMES!A1" display="ANTERIOR ⬅️" xr:uid="{407110AB-1511-4BF4-A89D-160684A83222}"/>
+    <hyperlink ref="C1" location="INFORMES!A1" display="ANTERIOR ⬅️" xr:uid="{407110AB-1511-4BF4-A89D-160684A83222}"/>
+    <hyperlink ref="D1" location="'BENS E DIREITOS'!A1" display="PRÓXIMO ➡️" xr:uid="{71F0E706-ABAF-4B50-82E9-9DADCADED2E3}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Despesa não identificada" error="Informe uma das categórias da lista" promptTitle="Informe a despesa" prompt="Informe uma das categórias da lista" xr:uid="{3F4AF9F4-3522-4151-B4E5-FC4CF549BBA4}">
+          <x14:formula1>
+            <xm:f>TABELAS!$C$2:$C$34</xm:f>
+          </x14:formula1>
+          <xm:sqref>H8:H48</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{477B38AF-3EA3-4F05-BB27-C33AF2D9B289}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="C1:I75"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="56" customWidth="1"/>
+    <col min="2" max="2" width="3.140625" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" customWidth="1"/>
+    <col min="4" max="4" width="43.7109375" customWidth="1"/>
+    <col min="5" max="6" width="25.7109375" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" customWidth="1"/>
+    <col min="8" max="9" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C3" s="27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C4" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+    </row>
+    <row r="6" spans="3:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="H6" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="I6" s="44" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C7" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="H7" s="45">
+        <f>SUM(E8:E18,E20:E28,E30:E34,E36:E42,E44:E48,E50:E53,E55:E60,E62:E68,E70:E75)</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="45">
+        <f>SUM(F8:F18,F20:F28,F30:F34,F36:F42,F44:F48,F50:F53,F55:F60,F62:F68,F70:F75)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C8" s="38"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C9" s="38"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C10" s="38"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="41"/>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C11" s="38"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="41"/>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C12" s="38"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="41"/>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C13" s="38"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="41"/>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C14" s="38"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="41"/>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C15" s="38"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="41"/>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C16" s="38"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="41"/>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C17" s="38"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="41"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C18" s="38"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="41"/>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C19" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C20" s="38"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="41"/>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C21" s="38"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="41"/>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C22" s="38"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="41"/>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C23" s="38"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C24" s="38"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C25" s="38"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C26" s="38"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C27" s="38"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C28" s="38"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C29" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C30" s="38"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C31" s="38"/>
+      <c r="D31" s="36"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C32" s="38"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+    </row>
+    <row r="33" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="38"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C34" s="38"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="41"/>
+    </row>
+    <row r="35" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="F35" s="28" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C36" s="38"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
+    </row>
+    <row r="37" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C37" s="38"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
+    </row>
+    <row r="38" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C38" s="38"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="41"/>
+    </row>
+    <row r="39" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C39" s="38"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="41"/>
+    </row>
+    <row r="40" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C40" s="38"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="41"/>
+      <c r="F40" s="41"/>
+    </row>
+    <row r="41" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C41" s="38"/>
+      <c r="D41" s="36"/>
+      <c r="E41" s="41"/>
+      <c r="F41" s="41"/>
+    </row>
+    <row r="42" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C42" s="38"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="41"/>
+      <c r="F42" s="41"/>
+    </row>
+    <row r="43" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C43" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="D43" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="E43" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="F43" s="28" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C44" s="38"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="41"/>
+      <c r="F44" s="41"/>
+    </row>
+    <row r="45" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C45" s="38"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="41"/>
+      <c r="F45" s="41"/>
+    </row>
+    <row r="46" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C46" s="38"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="41"/>
+    </row>
+    <row r="47" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C47" s="38"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
+    </row>
+    <row r="48" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C48" s="38"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="41"/>
+      <c r="F48" s="41"/>
+    </row>
+    <row r="49" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C49" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="D49" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="E49" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="F49" s="28" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C50" s="38"/>
+      <c r="D50" s="36"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="41"/>
+    </row>
+    <row r="51" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C51" s="38"/>
+      <c r="D51" s="36"/>
+      <c r="E51" s="41"/>
+      <c r="F51" s="41"/>
+    </row>
+    <row r="52" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C52" s="38"/>
+      <c r="D52" s="36"/>
+      <c r="E52" s="41"/>
+      <c r="F52" s="41"/>
+    </row>
+    <row r="53" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C53" s="38"/>
+      <c r="D53" s="36"/>
+      <c r="E53" s="41"/>
+      <c r="F53" s="41"/>
+    </row>
+    <row r="54" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C54" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="D54" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="E54" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="F54" s="28" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C55" s="38"/>
+      <c r="D55" s="36"/>
+      <c r="E55" s="41"/>
+      <c r="F55" s="41"/>
+    </row>
+    <row r="56" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C56" s="38"/>
+      <c r="D56" s="36"/>
+      <c r="E56" s="41"/>
+      <c r="F56" s="41"/>
+    </row>
+    <row r="57" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C57" s="38"/>
+      <c r="D57" s="36"/>
+      <c r="E57" s="41"/>
+      <c r="F57" s="41"/>
+    </row>
+    <row r="58" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C58" s="38"/>
+      <c r="D58" s="36"/>
+      <c r="E58" s="41"/>
+      <c r="F58" s="41"/>
+    </row>
+    <row r="59" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C59" s="38"/>
+      <c r="D59" s="36"/>
+      <c r="E59" s="41"/>
+      <c r="F59" s="41"/>
+    </row>
+    <row r="60" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C60" s="38"/>
+      <c r="D60" s="36"/>
+      <c r="E60" s="41"/>
+      <c r="F60" s="41"/>
+    </row>
+    <row r="61" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C61" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="D61" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="E61" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="F61" s="28" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="62" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C62" s="38"/>
+      <c r="D62" s="36"/>
+      <c r="E62" s="41"/>
+      <c r="F62" s="41"/>
+    </row>
+    <row r="63" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C63" s="38"/>
+      <c r="D63" s="36"/>
+      <c r="E63" s="41"/>
+      <c r="F63" s="41"/>
+    </row>
+    <row r="64" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C64" s="38"/>
+      <c r="D64" s="36"/>
+      <c r="E64" s="41"/>
+      <c r="F64" s="41"/>
+    </row>
+    <row r="65" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C65" s="38"/>
+      <c r="D65" s="36"/>
+      <c r="E65" s="41"/>
+      <c r="F65" s="41"/>
+    </row>
+    <row r="66" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C66" s="38"/>
+      <c r="D66" s="36"/>
+      <c r="E66" s="41"/>
+      <c r="F66" s="41"/>
+    </row>
+    <row r="67" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C67" s="38"/>
+      <c r="D67" s="36"/>
+      <c r="E67" s="41"/>
+      <c r="F67" s="41"/>
+    </row>
+    <row r="68" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C68" s="38"/>
+      <c r="D68" s="36"/>
+      <c r="E68" s="41"/>
+      <c r="F68" s="41"/>
+    </row>
+    <row r="69" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C69" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="D69" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="E69" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="F69" s="28" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="70" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C70" s="38"/>
+      <c r="D70" s="36"/>
+      <c r="E70" s="41"/>
+      <c r="F70" s="41"/>
+    </row>
+    <row r="71" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C71" s="38"/>
+      <c r="D71" s="36"/>
+      <c r="E71" s="41"/>
+      <c r="F71" s="41"/>
+    </row>
+    <row r="72" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C72" s="38"/>
+      <c r="D72" s="36"/>
+      <c r="E72" s="41">
+        <v>0</v>
+      </c>
+      <c r="F72" s="41"/>
+    </row>
+    <row r="73" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C73" s="38"/>
+      <c r="D73" s="36"/>
+      <c r="E73" s="41"/>
+      <c r="F73" s="41"/>
+    </row>
+    <row r="74" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C74" s="38"/>
+      <c r="D74" s="36"/>
+      <c r="E74" s="41"/>
+      <c r="F74" s="41"/>
+    </row>
+    <row r="75" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C75" s="38"/>
+      <c r="D75" s="36"/>
+      <c r="E75" s="41"/>
+      <c r="F75" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C6:F6"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E18 E30:E34 E20:E28 E36:E42 E44:E47" xr:uid="{B2265D1C-2258-4813-8275-F26F0A83B762}">
+      <formula1>"HOLHERITE,CNPJ,FREELANCE"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="C1" location="NOTAS!A1" display="ANTERIOR ⬅️" xr:uid="{0108452B-622A-4BB5-94D5-65729031DB2B}"/>
+  </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Item não corresponde" error="Selecione um item da lista" promptTitle="Selecione o Código" prompt="Selecione o Código correspondente" xr:uid="{550216CB-4150-4FCE-996E-BB364E5A57F5}">
+          <x14:formula1>
+            <xm:f>TABELAS!$E$3:$E$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>C8:C18</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Item não corresponde" error="Selecione um item da lista" promptTitle="Selecione o Código" prompt="Selecione o Código correspondente" xr:uid="{B91762DC-6E82-45D9-A55D-3D8089E32344}">
+          <x14:formula1>
+            <xm:f>TABELAS!$E$12:$E$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>C20:C28</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Item não corresponde" error="Selecione um item da lista" promptTitle="Selecione o Código" prompt="Selecione o Código correspondente" xr:uid="{EF9ACF4D-CE15-4502-847F-068A1F672122}">
+          <x14:formula1>
+            <xm:f>TABELAS!$E$18:$E$20</xm:f>
+          </x14:formula1>
+          <xm:sqref>C30:C34</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Item não corresponde" error="Selecione um item da lista" promptTitle="Selecione o Código" prompt="Selecione o Código correspondente" xr:uid="{FEF8F248-AC8A-4158-AD8B-6E0F7B1C8D25}">
+          <x14:formula1>
+            <xm:f>TABELAS!$E$23:$E$29</xm:f>
+          </x14:formula1>
+          <xm:sqref>C36:C42</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Item não corresponde" error="Selecione um item da lista" promptTitle="Selecione o Código" prompt="Selecione o Código correspondente" xr:uid="{E0B9C168-A410-478F-95E5-8471EBD43B15}">
+          <x14:formula1>
+            <xm:f>TABELAS!$E$32:$E$34</xm:f>
+          </x14:formula1>
+          <xm:sqref>C44:C48</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Item não corresponde" error="Selecione um item da lista" promptTitle="Selecione o Código" prompt="Selecione o Código correspondente" xr:uid="{99C7DA76-29C6-4832-ACC4-E4BB5D1E0E16}">
+          <x14:formula1>
+            <xm:f>TABELAS!$E$37:$E$39</xm:f>
+          </x14:formula1>
+          <xm:sqref>C50:C53</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Item não corresponde" error="Selecione um item da lista" promptTitle="Selecione o Código" prompt="Selecione o Código correspondente" xr:uid="{D1E954E4-068E-4AF7-BB47-0B275C12C020}">
+          <x14:formula1>
+            <xm:f>TABELAS!$E$42:$E$45</xm:f>
+          </x14:formula1>
+          <xm:sqref>C55:C60</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Item não corresponde" error="Selecione um item da lista" promptTitle="Selecione o Código" prompt="Selecione o Código correspondente" xr:uid="{598A37CD-26B5-488D-98E7-ECD31A8008BC}">
+          <x14:formula1>
+            <xm:f>TABELAS!$E$48:$E$51</xm:f>
+          </x14:formula1>
+          <xm:sqref>C62:C68</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Item não corresponde" error="Selecione um item da lista" promptTitle="Selecione o Código" prompt="Selecione o Código correspondente" xr:uid="{A32B6F5A-A2CF-4F1B-A1BA-759F0509FCA9}">
+          <x14:formula1>
+            <xm:f>TABELAS!$E$54:$E$58</xm:f>
+          </x14:formula1>
+          <xm:sqref>C70:C75</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C12BCAF-3F1C-4962-B8E7-F7B02808735E}">
-  <dimension ref="A1:A49"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="62.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.7109375" customWidth="1"/>
+    <col min="3" max="3" width="79.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="C1" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
+      <c r="C2" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="43" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
+      <c r="C3" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="18" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+      <c r="C4" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="C5" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+      <c r="C6" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="19" t="s">
+      <c r="C7" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+      <c r="C8" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
+      <c r="C9" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
+      <c r="C10" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="19" t="s">
+      <c r="C11" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="18" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
+      <c r="C12" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="18" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="19" t="s">
+      <c r="C13" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="19" t="s">
+      <c r="C14" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="19" t="s">
+      <c r="C15" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
+      <c r="C16" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
+      <c r="C17" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" s="43" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
+      <c r="C18" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="18" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="19" t="s">
+      <c r="C19" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="18" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="19" t="s">
+      <c r="C20" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="18" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="19" t="s">
+      <c r="C21" s="18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="18" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="19" t="s">
+      <c r="C22" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" s="43" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="18" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="19" t="s">
+      <c r="C23" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="18" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="19" t="s">
+      <c r="C24" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="18" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="19" t="s">
+      <c r="C25" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="18" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="19" t="s">
+      <c r="C26" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="18" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="19" t="s">
+      <c r="C27" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="19" t="s">
+      <c r="C28" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="18" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="19" t="s">
+      <c r="C29" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="18" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="19" t="s">
+      <c r="C30" s="18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="18" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="19" t="s">
+      <c r="C31" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="E31" s="43" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="18" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="19" t="s">
+      <c r="C32" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="18" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="19" t="s">
+      <c r="C33" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="19" t="s">
+      <c r="C34" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="19" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="18" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="19" t="s">
+      <c r="E36" s="43" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="18" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="19" t="s">
+      <c r="E37" s="18" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="18" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="19" t="s">
+      <c r="E38" s="18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="19" t="s">
+      <c r="E39" s="18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="18" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="19" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="18" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="19" t="s">
+      <c r="E41" s="43" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="18" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="19" t="s">
+      <c r="E42" s="18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="18" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="19" t="s">
+      <c r="E43" s="18" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="18" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="19" t="s">
+      <c r="E44" s="18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="18" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="19" t="s">
+      <c r="E45" s="18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="18" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="19" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="18" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="19" t="s">
+      <c r="E47" s="43" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="18" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="19" t="s">
+      <c r="E48" s="18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="18" t="s">
         <v>72</v>
+      </c>
+      <c r="E49" s="18" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E50" s="18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E51" s="18" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E53" s="43" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E54" s="18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E55" s="18" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E56" s="18" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E57" s="18" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E58" s="18" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>